<commit_message>
AG-add clean QC functions script, DA-file organization
</commit_message>
<xml_diff>
--- a/inst/TaskList.xlsx
+++ b/inst/TaskList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Explicitly note what problems exist in each one of the example datasets</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -490,6 +493,15 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
issue with cleaned data save
</commit_message>
<xml_diff>
--- a/inst/TaskList.xlsx
+++ b/inst/TaskList.xlsx
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Include sampleID and Param in message to user</t>
   </si>
   <si>
     <t>Check for characters in results column</t>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Needs testing as of 1/20/26</t>
+  </si>
+  <si>
+    <t>within flag_below_lod() there is coercion to numeric which will warn about NA's being introduced</t>
   </si>
 </sst>
 </file>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -608,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -628,10 +628,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2">
         <v>46042</v>
@@ -645,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -653,22 +653,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2">
         <v>46042</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -676,16 +676,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2">
         <v>46042</v>
@@ -696,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -704,50 +704,50 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
         <v>46042</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -755,22 +755,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F10" s="2">
         <v>46042</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -786,36 +786,36 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2">
         <v>46042</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -823,22 +823,22 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="2">
         <v>46042</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -846,22 +846,22 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2">
         <v>46042</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -869,19 +869,19 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>